<commit_message>
Formatting DSS data + minor code modifications
</commit_message>
<xml_diff>
--- a/adult-DSS-exp4/Classeur1.xlsx
+++ b/adult-DSS-exp4/Classeur1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\Chercheurs\Santos_Manuela\Thibault M\gut-microbiota-iron\adult-DSS-exp4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{50AA03DE-5BC5-4588-9C1B-D44381CEAFA6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7315C3A-A0AF-45D1-96AE-B229B35B5FA1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11625" xr2:uid="{45985671-1A5D-4E30-93E9-71AD4CA4C8CC}"/>
   </bookViews>
@@ -310,10 +310,17 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0" tint="-0.34998626667073579"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -456,7 +463,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -475,6 +482,18 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -789,15 +808,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92C7ADD1-5593-40A9-A9DC-5D15A6AAF184}">
-  <dimension ref="A1:J70"/>
+  <dimension ref="A1:L70"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+      <selection activeCell="L1" sqref="L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>86</v>
       </c>
@@ -818,220 +837,223 @@
       </c>
       <c r="J1" s="17">
         <f ca="1">TODAY()</f>
-        <v>45442</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
+        <v>45453</v>
+      </c>
+      <c r="L1" s="17">
+        <v>45462</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="18">
         <v>268420</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="3">
+      <c r="C2" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="20">
         <v>45374</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="4">
-        <f ca="1">(J$1-D2)/7</f>
-        <v>9.7142857142857135</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="5">
+      <c r="F2" s="21">
+        <f t="shared" ref="F2:H33" ca="1" si="0">(J$1-D2)/7</f>
+        <v>11.285714285714286</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="22">
         <v>268420</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" s="7">
+      <c r="C3" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="24">
         <v>45374</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="8">
-        <f ca="1">(J$1-D3)/7</f>
-        <v>9.7142857142857135</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="5">
+      <c r="F3" s="25">
+        <f t="shared" ca="1" si="0"/>
+        <v>11.285714285714286</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="22">
         <v>268420</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="D4" s="7">
+      <c r="C4" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="24">
         <v>45374</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="E4" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="8">
-        <f ca="1">(J$1-D4)/7</f>
-        <v>9.7142857142857135</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="5">
+      <c r="F4" s="25">
+        <f t="shared" ca="1" si="0"/>
+        <v>11.285714285714286</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="22">
         <v>268420</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="D5" s="7">
+      <c r="C5" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" s="24">
         <v>45374</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="E5" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="F5" s="8">
-        <f ca="1">(J$1-D5)/7</f>
-        <v>9.7142857142857135</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="9">
+      <c r="F5" s="25">
+        <f t="shared" ca="1" si="0"/>
+        <v>11.285714285714286</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="26">
         <v>268420</v>
       </c>
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="D6" s="11">
+      <c r="C6" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="D6" s="28">
         <v>45374</v>
       </c>
-      <c r="E6" s="10" t="s">
+      <c r="E6" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="F6" s="12">
-        <f ca="1">(J$1-D6)/7</f>
-        <v>9.7142857142857135</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
+      <c r="F6" s="29">
+        <f t="shared" ca="1" si="0"/>
+        <v>11.285714285714286</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="18">
         <v>268646</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D7" s="3">
+      <c r="C7" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="D7" s="20">
         <v>45378</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="E7" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="F7" s="4">
-        <f ca="1">(J$1-D7)/7</f>
-        <v>9.1428571428571423</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="5">
+      <c r="F7" s="21">
+        <f t="shared" ca="1" si="0"/>
+        <v>10.714285714285714</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" s="22">
         <v>268646</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="D8" s="7">
+      <c r="C8" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="D8" s="24">
         <v>45378</v>
       </c>
-      <c r="E8" s="6" t="s">
+      <c r="E8" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="F8" s="8">
-        <f ca="1">(J$1-D8)/7</f>
-        <v>9.1428571428571423</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="9">
+      <c r="F8" s="25">
+        <f t="shared" ca="1" si="0"/>
+        <v>10.714285714285714</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="26">
         <v>268646</v>
       </c>
-      <c r="B9" s="10" t="s">
+      <c r="B9" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="D9" s="11">
+      <c r="C9" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="D9" s="28">
         <v>45378</v>
       </c>
-      <c r="E9" s="10" t="s">
+      <c r="E9" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="F9" s="12">
-        <f ca="1">(J$1-D9)/7</f>
-        <v>9.1428571428571423</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
+      <c r="F9" s="29">
+        <f t="shared" ca="1" si="0"/>
+        <v>10.714285714285714</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" s="18">
         <v>269007</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D10" s="3">
+      <c r="C10" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="D10" s="20">
         <v>45376</v>
       </c>
-      <c r="E10" s="2" t="s">
+      <c r="E10" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="F10" s="4">
-        <f ca="1">(J$1-D10)/7</f>
-        <v>9.4285714285714288</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="9">
+      <c r="F10" s="21">
+        <f t="shared" ca="1" si="0"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="26">
         <v>269007</v>
       </c>
-      <c r="B11" s="10" t="s">
+      <c r="B11" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="C11" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="D11" s="11">
+      <c r="C11" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="D11" s="28">
         <v>45376</v>
       </c>
-      <c r="E11" s="10" t="s">
+      <c r="E11" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="F11" s="12">
-        <f ca="1">(J$1-D11)/7</f>
-        <v>9.4285714285714288</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F11" s="29">
+        <f t="shared" ca="1" si="0"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>269060</v>
       </c>
@@ -1048,14 +1070,18 @@
         <v>2</v>
       </c>
       <c r="F12" s="4">
-        <f ca="1">(J$1-D12)/7</f>
-        <v>8.5714285714285712</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>10.142857142857142</v>
       </c>
       <c r="G12">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H12" s="4">
+        <f>(L$1-D12)/7</f>
+        <v>11.428571428571429</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="9">
         <v>269060</v>
       </c>
@@ -1072,14 +1098,18 @@
         <v>2</v>
       </c>
       <c r="F13" s="12">
-        <f ca="1">(J$1-D13)/7</f>
-        <v>8.5714285714285712</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>10.142857142857142</v>
       </c>
       <c r="G13">
         <v>2</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H13" s="4">
+        <f t="shared" ref="H13:H70" si="1">(L$1-D13)/7</f>
+        <v>11.428571428571429</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>269136</v>
       </c>
@@ -1096,14 +1126,18 @@
         <v>17</v>
       </c>
       <c r="F14" s="4">
-        <f ca="1">(J$1-D14)/7</f>
-        <v>8.5714285714285712</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>10.142857142857142</v>
       </c>
       <c r="G14">
         <v>3</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H14" s="4">
+        <f t="shared" si="1"/>
+        <v>11.428571428571429</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="5">
         <v>269136</v>
       </c>
@@ -1120,14 +1154,18 @@
         <v>17</v>
       </c>
       <c r="F15" s="8">
-        <f ca="1">(J$1-D15)/7</f>
-        <v>8.5714285714285712</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>10.142857142857142</v>
       </c>
       <c r="G15">
         <v>4</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H15" s="4">
+        <f t="shared" si="1"/>
+        <v>11.428571428571429</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="5">
         <v>269136</v>
       </c>
@@ -1144,14 +1182,18 @@
         <v>17</v>
       </c>
       <c r="F16" s="8">
-        <f ca="1">(J$1-D16)/7</f>
-        <v>8.5714285714285712</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>10.142857142857142</v>
       </c>
       <c r="G16">
         <v>5</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H16" s="4">
+        <f t="shared" si="1"/>
+        <v>11.428571428571429</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="5">
         <v>269136</v>
       </c>
@@ -1168,14 +1210,18 @@
         <v>17</v>
       </c>
       <c r="F17" s="8">
-        <f ca="1">(J$1-D17)/7</f>
-        <v>8.5714285714285712</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>10.142857142857142</v>
       </c>
       <c r="G17">
         <v>6</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H17" s="4">
+        <f t="shared" si="1"/>
+        <v>11.428571428571429</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="9">
         <v>269136</v>
       </c>
@@ -1192,14 +1238,18 @@
         <v>17</v>
       </c>
       <c r="F18" s="12">
-        <f ca="1">(J$1-D18)/7</f>
-        <v>8.5714285714285712</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>10.142857142857142</v>
       </c>
       <c r="G18">
         <v>7</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H18" s="4">
+        <f t="shared" si="1"/>
+        <v>11.428571428571429</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>269137</v>
       </c>
@@ -1216,14 +1266,18 @@
         <v>23</v>
       </c>
       <c r="F19" s="4">
-        <f ca="1">(J$1-D19)/7</f>
-        <v>8.5714285714285712</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>10.142857142857142</v>
       </c>
       <c r="G19">
         <v>8</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H19" s="4">
+        <f t="shared" si="1"/>
+        <v>11.428571428571429</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="5">
         <v>269137</v>
       </c>
@@ -1240,14 +1294,18 @@
         <v>23</v>
       </c>
       <c r="F20" s="8">
-        <f ca="1">(J$1-D20)/7</f>
-        <v>8.5714285714285712</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>10.142857142857142</v>
       </c>
       <c r="G20">
         <v>9</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H20" s="4">
+        <f t="shared" si="1"/>
+        <v>11.428571428571429</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="9">
         <v>269137</v>
       </c>
@@ -1264,14 +1322,18 @@
         <v>23</v>
       </c>
       <c r="F21" s="12">
-        <f ca="1">(J$1-D21)/7</f>
-        <v>8.5714285714285712</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>10.142857142857142</v>
       </c>
       <c r="G21">
         <v>10</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H21" s="4">
+        <f t="shared" si="1"/>
+        <v>11.428571428571429</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>269160</v>
       </c>
@@ -1288,14 +1350,18 @@
         <v>27</v>
       </c>
       <c r="F22" s="4">
-        <f ca="1">(J$1-D22)/7</f>
-        <v>8.1428571428571423</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>9.7142857142857135</v>
       </c>
       <c r="G22">
+        <v>1</v>
+      </c>
+      <c r="H22" s="4">
+        <f t="shared" si="1"/>
         <v>11</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="5">
         <v>269160</v>
       </c>
@@ -1312,14 +1378,18 @@
         <v>27</v>
       </c>
       <c r="F23" s="8">
-        <f ca="1">(J$1-D23)/7</f>
-        <v>8.1428571428571423</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>9.7142857142857135</v>
       </c>
       <c r="G23">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="H23" s="4">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="5">
         <v>269160</v>
       </c>
@@ -1336,14 +1406,18 @@
         <v>27</v>
       </c>
       <c r="F24" s="8">
-        <f ca="1">(J$1-D24)/7</f>
-        <v>8.1428571428571423</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>9.7142857142857135</v>
       </c>
       <c r="G24">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="H24" s="4">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="5">
         <v>269160</v>
       </c>
@@ -1360,14 +1434,18 @@
         <v>27</v>
       </c>
       <c r="F25" s="8">
-        <f ca="1">(J$1-D25)/7</f>
-        <v>8.1428571428571423</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>9.7142857142857135</v>
       </c>
       <c r="G25">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>4</v>
+      </c>
+      <c r="H25" s="4">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="9">
         <v>269160</v>
       </c>
@@ -1384,14 +1462,18 @@
         <v>27</v>
       </c>
       <c r="F26" s="12">
-        <f ca="1">(J$1-D26)/7</f>
-        <v>8.1428571428571423</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>9.7142857142857135</v>
       </c>
       <c r="G26">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+      <c r="H26" s="4">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>269703</v>
       </c>
@@ -1408,14 +1490,18 @@
         <v>33</v>
       </c>
       <c r="F27" s="4">
-        <f ca="1">(J$1-D27)/7</f>
-        <v>7.4285714285714288</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>9</v>
       </c>
       <c r="G27">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>6</v>
+      </c>
+      <c r="H27" s="4">
+        <f t="shared" si="1"/>
+        <v>10.285714285714286</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="9">
         <v>269703</v>
       </c>
@@ -1432,14 +1518,18 @@
         <v>33</v>
       </c>
       <c r="F28" s="12">
-        <f ca="1">(J$1-D28)/7</f>
-        <v>7.4285714285714288</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>9</v>
       </c>
       <c r="G28">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+      <c r="H28" s="4">
+        <f t="shared" si="1"/>
+        <v>10.285714285714286</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <v>269707</v>
       </c>
@@ -1456,14 +1546,18 @@
         <v>36</v>
       </c>
       <c r="F29" s="4">
-        <f ca="1">(J$1-D29)/7</f>
-        <v>7</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>8.5714285714285712</v>
       </c>
       <c r="G29">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>8</v>
+      </c>
+      <c r="H29" s="4">
+        <f t="shared" si="1"/>
+        <v>9.8571428571428577</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="9">
         <v>269707</v>
       </c>
@@ -1480,14 +1574,18 @@
         <v>36</v>
       </c>
       <c r="F30" s="12">
-        <f ca="1">(J$1-D30)/7</f>
-        <v>7</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>8.5714285714285712</v>
       </c>
       <c r="G30">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+      <c r="H30" s="4">
+        <f t="shared" si="1"/>
+        <v>9.8571428571428577</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
         <v>269709</v>
       </c>
@@ -1504,14 +1602,18 @@
         <v>39</v>
       </c>
       <c r="F31" s="4">
-        <f ca="1">(J$1-D31)/7</f>
-        <v>7</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>8.5714285714285712</v>
       </c>
       <c r="G31">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+      <c r="H31" s="4">
+        <f t="shared" si="1"/>
+        <v>9.8571428571428577</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="9">
         <v>269709</v>
       </c>
@@ -1528,14 +1630,18 @@
         <v>39</v>
       </c>
       <c r="F32" s="12">
-        <f ca="1">(J$1-D32)/7</f>
-        <v>7</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>8.5714285714285712</v>
       </c>
       <c r="G32">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+      <c r="H32" s="4">
+        <f t="shared" si="1"/>
+        <v>9.8571428571428577</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="1">
         <v>269711</v>
       </c>
@@ -1552,14 +1658,18 @@
         <v>42</v>
       </c>
       <c r="F33" s="4">
-        <f ca="1">(J$1-D33)/7</f>
-        <v>6.8571428571428568</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>8.4285714285714288</v>
       </c>
       <c r="G33">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>12</v>
+      </c>
+      <c r="H33" s="4">
+        <f t="shared" si="1"/>
+        <v>9.7142857142857135</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="9">
         <v>269711</v>
       </c>
@@ -1576,14 +1686,18 @@
         <v>42</v>
       </c>
       <c r="F34" s="12">
-        <f ca="1">(J$1-D34)/7</f>
-        <v>6.8571428571428568</v>
+        <f t="shared" ref="F34:F70" ca="1" si="2">(J$1-D34)/7</f>
+        <v>8.4285714285714288</v>
       </c>
       <c r="G34">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+      <c r="H34" s="4">
+        <f t="shared" si="1"/>
+        <v>9.7142857142857135</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="1">
         <v>269713</v>
       </c>
@@ -1600,14 +1714,18 @@
         <v>45</v>
       </c>
       <c r="F35" s="4">
-        <f ca="1">(J$1-D35)/7</f>
-        <v>6.7142857142857144</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>8.2857142857142865</v>
       </c>
       <c r="G35">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+      <c r="H35" s="4">
+        <f t="shared" si="1"/>
+        <v>9.5714285714285712</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="5">
         <v>269713</v>
       </c>
@@ -1624,14 +1742,18 @@
         <v>45</v>
       </c>
       <c r="F36" s="8">
-        <f ca="1">(J$1-D36)/7</f>
-        <v>6.7142857142857144</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>8.2857142857142865</v>
       </c>
       <c r="G36">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+      <c r="H36" s="4">
+        <f t="shared" si="1"/>
+        <v>9.5714285714285712</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="5">
         <v>269713</v>
       </c>
@@ -1648,14 +1770,18 @@
         <v>45</v>
       </c>
       <c r="F37" s="8">
-        <f ca="1">(J$1-D37)/7</f>
-        <v>6.7142857142857144</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>8.2857142857142865</v>
       </c>
       <c r="G37">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>16</v>
+      </c>
+      <c r="H37" s="4">
+        <f t="shared" si="1"/>
+        <v>9.5714285714285712</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="9">
         <v>269713</v>
       </c>
@@ -1672,14 +1798,18 @@
         <v>45</v>
       </c>
       <c r="F38" s="12">
-        <f ca="1">(J$1-D38)/7</f>
-        <v>6.7142857142857144</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>8.2857142857142865</v>
       </c>
       <c r="G38">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>17</v>
+      </c>
+      <c r="H38" s="4">
+        <f t="shared" si="1"/>
+        <v>9.5714285714285712</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="13">
         <v>270133</v>
       </c>
@@ -1696,14 +1826,18 @@
         <v>50</v>
       </c>
       <c r="F39" s="16">
-        <f ca="1">(J$1-D39)/7</f>
-        <v>6.5714285714285712</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>8.1428571428571423</v>
       </c>
       <c r="G39">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+      <c r="H39" s="4">
+        <f t="shared" si="1"/>
+        <v>9.4285714285714288</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="1">
         <v>270374</v>
       </c>
@@ -1720,14 +1854,18 @@
         <v>2</v>
       </c>
       <c r="F40" s="4">
-        <f ca="1">(J$1-D40)/7</f>
-        <v>5.8571428571428568</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>7.4285714285714288</v>
       </c>
       <c r="G40">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+      <c r="H40" s="4">
+        <f t="shared" si="1"/>
+        <v>8.7142857142857135</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="5">
         <v>270374</v>
       </c>
@@ -1744,14 +1882,18 @@
         <v>2</v>
       </c>
       <c r="F41" s="8">
-        <f ca="1">(J$1-D41)/7</f>
-        <v>5.8571428571428568</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>7.4285714285714288</v>
       </c>
       <c r="G41">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+      <c r="H41" s="4">
+        <f t="shared" si="1"/>
+        <v>8.7142857142857135</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="5">
         <v>270374</v>
       </c>
@@ -1768,14 +1910,18 @@
         <v>2</v>
       </c>
       <c r="F42" s="8">
-        <f ca="1">(J$1-D42)/7</f>
-        <v>5.8571428571428568</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>7.4285714285714288</v>
       </c>
       <c r="G42">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+      <c r="H42" s="4">
+        <f t="shared" si="1"/>
+        <v>8.7142857142857135</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="5">
         <v>270374</v>
       </c>
@@ -1792,14 +1938,18 @@
         <v>2</v>
       </c>
       <c r="F43" s="8">
-        <f ca="1">(J$1-D43)/7</f>
-        <v>5.8571428571428568</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>7.4285714285714288</v>
       </c>
       <c r="G43">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>22</v>
+      </c>
+      <c r="H43" s="4">
+        <f t="shared" si="1"/>
+        <v>8.7142857142857135</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="9">
         <v>270374</v>
       </c>
@@ -1816,14 +1966,18 @@
         <v>2</v>
       </c>
       <c r="F44" s="12">
-        <f ca="1">(J$1-D44)/7</f>
-        <v>5.8571428571428568</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>7.4285714285714288</v>
       </c>
       <c r="G44">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>23</v>
+      </c>
+      <c r="H44" s="4">
+        <f t="shared" si="1"/>
+        <v>8.7142857142857135</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="13">
         <v>270386</v>
       </c>
@@ -1840,14 +1994,18 @@
         <v>57</v>
       </c>
       <c r="F45" s="16">
-        <f ca="1">(J$1-D45)/7</f>
-        <v>6.4285714285714288</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>8</v>
       </c>
       <c r="G45">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+      <c r="H45" s="4">
+        <f t="shared" si="1"/>
+        <v>9.2857142857142865</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="1">
         <v>270388</v>
       </c>
@@ -1864,14 +2022,18 @@
         <v>8</v>
       </c>
       <c r="F46" s="4">
-        <f ca="1">(J$1-D46)/7</f>
-        <v>6</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>7.5714285714285712</v>
       </c>
       <c r="G46">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+      <c r="H46" s="4">
+        <f t="shared" si="1"/>
+        <v>8.8571428571428577</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="5">
         <v>270388</v>
       </c>
@@ -1888,14 +2050,18 @@
         <v>8</v>
       </c>
       <c r="F47" s="8">
-        <f ca="1">(J$1-D47)/7</f>
-        <v>6</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>7.5714285714285712</v>
       </c>
       <c r="G47">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+      <c r="H47" s="4">
+        <f t="shared" si="1"/>
+        <v>8.8571428571428577</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="9">
         <v>270388</v>
       </c>
@@ -1912,14 +2078,18 @@
         <v>8</v>
       </c>
       <c r="F48" s="12">
-        <f ca="1">(J$1-D48)/7</f>
-        <v>6</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>7.5714285714285712</v>
       </c>
       <c r="G48">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+      <c r="H48" s="4">
+        <f t="shared" si="1"/>
+        <v>8.8571428571428577</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="1">
         <v>270752</v>
       </c>
@@ -1936,14 +2106,18 @@
         <v>62</v>
       </c>
       <c r="F49" s="4">
-        <f ca="1">(J$1-D49)/7</f>
-        <v>5.4285714285714288</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>7</v>
       </c>
       <c r="G49">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+      <c r="H49" s="4">
+        <f t="shared" si="1"/>
+        <v>8.2857142857142865</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="5">
         <v>270752</v>
       </c>
@@ -1960,14 +2134,18 @@
         <v>62</v>
       </c>
       <c r="F50" s="8">
-        <f ca="1">(J$1-D50)/7</f>
-        <v>5.4285714285714288</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>7</v>
       </c>
       <c r="G50">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>29</v>
+      </c>
+      <c r="H50" s="4">
+        <f t="shared" si="1"/>
+        <v>8.2857142857142865</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="9">
         <v>270752</v>
       </c>
@@ -1984,14 +2162,18 @@
         <v>62</v>
       </c>
       <c r="F51" s="12">
-        <f ca="1">(J$1-D51)/7</f>
-        <v>5.4285714285714288</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>7</v>
       </c>
       <c r="G51">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+      <c r="H51" s="4">
+        <f t="shared" si="1"/>
+        <v>8.2857142857142865</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="1">
         <v>270754</v>
       </c>
@@ -2008,14 +2190,18 @@
         <v>39</v>
       </c>
       <c r="F52" s="4">
-        <f ca="1">(J$1-D52)/7</f>
-        <v>5.2857142857142856</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>6.8571428571428568</v>
       </c>
       <c r="G52">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+      <c r="H52" s="4">
+        <f t="shared" si="1"/>
+        <v>8.1428571428571423</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="5">
         <v>270754</v>
       </c>
@@ -2032,14 +2218,18 @@
         <v>39</v>
       </c>
       <c r="F53" s="8">
-        <f ca="1">(J$1-D53)/7</f>
-        <v>5.2857142857142856</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>6.8571428571428568</v>
       </c>
       <c r="G53">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+      <c r="H53" s="4">
+        <f t="shared" si="1"/>
+        <v>8.1428571428571423</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="5">
         <v>270754</v>
       </c>
@@ -2056,14 +2246,18 @@
         <v>39</v>
       </c>
       <c r="F54" s="8">
-        <f ca="1">(J$1-D54)/7</f>
-        <v>5.2857142857142856</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>6.8571428571428568</v>
       </c>
       <c r="G54">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+      <c r="H54" s="4">
+        <f t="shared" si="1"/>
+        <v>8.1428571428571423</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="5">
         <v>270754</v>
       </c>
@@ -2080,14 +2274,18 @@
         <v>39</v>
       </c>
       <c r="F55" s="8">
-        <f ca="1">(J$1-D55)/7</f>
-        <v>5.2857142857142856</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>6.8571428571428568</v>
       </c>
       <c r="G55">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>34</v>
+      </c>
+      <c r="H55" s="4">
+        <f t="shared" si="1"/>
+        <v>8.1428571428571423</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="9">
         <v>270754</v>
       </c>
@@ -2104,14 +2302,18 @@
         <v>39</v>
       </c>
       <c r="F56" s="12">
-        <f ca="1">(J$1-D56)/7</f>
-        <v>5.2857142857142856</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>6.8571428571428568</v>
       </c>
       <c r="G56">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+      <c r="H56" s="4">
+        <f t="shared" si="1"/>
+        <v>8.1428571428571423</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A57" s="1">
         <v>270758</v>
       </c>
@@ -2128,14 +2330,18 @@
         <v>27</v>
       </c>
       <c r="F57" s="4">
-        <f ca="1">(J$1-D57)/7</f>
-        <v>5</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>6.5714285714285712</v>
       </c>
       <c r="G57">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="58" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>36</v>
+      </c>
+      <c r="H57" s="4">
+        <f t="shared" si="1"/>
+        <v>7.8571428571428568</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" s="9">
         <v>270758</v>
       </c>
@@ -2152,14 +2358,18 @@
         <v>27</v>
       </c>
       <c r="F58" s="12">
-        <f ca="1">(J$1-D58)/7</f>
-        <v>5</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>6.5714285714285712</v>
       </c>
       <c r="G58">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+      <c r="H58" s="4">
+        <f t="shared" si="1"/>
+        <v>7.8571428571428568</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A59" s="1">
         <v>270760</v>
       </c>
@@ -2176,11 +2386,18 @@
         <v>73</v>
       </c>
       <c r="F59" s="4">
-        <f ca="1">(J$1-D59)/7</f>
-        <v>4.7142857142857144</v>
-      </c>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="2"/>
+        <v>6.2857142857142856</v>
+      </c>
+      <c r="G59">
+        <v>38</v>
+      </c>
+      <c r="H59" s="4">
+        <f t="shared" si="1"/>
+        <v>7.5714285714285712</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A60" s="5">
         <v>270760</v>
       </c>
@@ -2197,11 +2414,18 @@
         <v>73</v>
       </c>
       <c r="F60" s="8">
-        <f ca="1">(J$1-D60)/7</f>
-        <v>4.7142857142857144</v>
-      </c>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="2"/>
+        <v>6.2857142857142856</v>
+      </c>
+      <c r="G60">
+        <v>39</v>
+      </c>
+      <c r="H60" s="4">
+        <f t="shared" si="1"/>
+        <v>7.5714285714285712</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A61" s="5">
         <v>270760</v>
       </c>
@@ -2218,11 +2442,18 @@
         <v>73</v>
       </c>
       <c r="F61" s="8">
-        <f ca="1">(J$1-D61)/7</f>
-        <v>4.7142857142857144</v>
-      </c>
-    </row>
-    <row r="62" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <f t="shared" ca="1" si="2"/>
+        <v>6.2857142857142856</v>
+      </c>
+      <c r="G61">
+        <v>40</v>
+      </c>
+      <c r="H61" s="4">
+        <f t="shared" si="1"/>
+        <v>7.5714285714285712</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A62" s="9">
         <v>270760</v>
       </c>
@@ -2240,10 +2471,17 @@
       </c>
       <c r="F62" s="12">
         <f ca="1">(J$1-D62)/7</f>
-        <v>4.7142857142857144</v>
-      </c>
-    </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+        <v>6.2857142857142856</v>
+      </c>
+      <c r="G62">
+        <v>41</v>
+      </c>
+      <c r="H62" s="4">
+        <f t="shared" si="1"/>
+        <v>7.5714285714285712</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A63" s="1">
         <v>270761</v>
       </c>
@@ -2260,11 +2498,18 @@
         <v>73</v>
       </c>
       <c r="F63" s="4">
-        <f ca="1">(J$1-D63)/7</f>
-        <v>4.7142857142857144</v>
-      </c>
-    </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="2"/>
+        <v>6.2857142857142856</v>
+      </c>
+      <c r="G63">
+        <v>42</v>
+      </c>
+      <c r="H63" s="4">
+        <f t="shared" si="1"/>
+        <v>7.5714285714285712</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A64" s="5">
         <v>270761</v>
       </c>
@@ -2281,11 +2526,18 @@
         <v>73</v>
       </c>
       <c r="F64" s="8">
-        <f ca="1">(J$1-D64)/7</f>
-        <v>4.7142857142857144</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <f t="shared" ca="1" si="2"/>
+        <v>6.2857142857142856</v>
+      </c>
+      <c r="G64">
+        <v>43</v>
+      </c>
+      <c r="H64" s="4">
+        <f t="shared" si="1"/>
+        <v>7.5714285714285712</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A65" s="9">
         <v>270761</v>
       </c>
@@ -2302,11 +2554,18 @@
         <v>73</v>
       </c>
       <c r="F65" s="12">
-        <f ca="1">(J$1-D65)/7</f>
-        <v>4.7142857142857144</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="2"/>
+        <v>6.2857142857142856</v>
+      </c>
+      <c r="G65">
+        <v>44</v>
+      </c>
+      <c r="H65" s="4">
+        <f t="shared" si="1"/>
+        <v>7.5714285714285712</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A66" s="1">
         <v>271387</v>
       </c>
@@ -2323,11 +2582,18 @@
         <v>81</v>
       </c>
       <c r="F66" s="4">
-        <f ca="1">(J$1-D66)/7</f>
-        <v>4.4285714285714288</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="G66">
+        <v>45</v>
+      </c>
+      <c r="H66" s="4">
+        <f>(L$1-D66)/7</f>
+        <v>7.2857142857142856</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A67" s="5">
         <v>271387</v>
       </c>
@@ -2344,11 +2610,18 @@
         <v>81</v>
       </c>
       <c r="F67" s="8">
-        <f ca="1">(J$1-D67)/7</f>
-        <v>4.4285714285714288</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="G67">
+        <v>46</v>
+      </c>
+      <c r="H67" s="4">
+        <f t="shared" si="1"/>
+        <v>7.2857142857142856</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A68" s="5">
         <v>271387</v>
       </c>
@@ -2365,11 +2638,18 @@
         <v>81</v>
       </c>
       <c r="F68" s="8">
-        <f ca="1">(J$1-D68)/7</f>
-        <v>4.4285714285714288</v>
-      </c>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="G68">
+        <v>47</v>
+      </c>
+      <c r="H68" s="4">
+        <f t="shared" si="1"/>
+        <v>7.2857142857142856</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A69" s="5">
         <v>271387</v>
       </c>
@@ -2386,11 +2666,18 @@
         <v>81</v>
       </c>
       <c r="F69" s="8">
-        <f ca="1">(J$1-D69)/7</f>
-        <v>4.4285714285714288</v>
-      </c>
-    </row>
-    <row r="70" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <f t="shared" ca="1" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="G69">
+        <v>48</v>
+      </c>
+      <c r="H69" s="4">
+        <f t="shared" si="1"/>
+        <v>7.2857142857142856</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A70" s="9">
         <v>271387</v>
       </c>
@@ -2407,11 +2694,19 @@
         <v>81</v>
       </c>
       <c r="F70" s="12">
-        <f ca="1">(J$1-D70)/7</f>
-        <v>4.4285714285714288</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="G70">
+        <v>49</v>
+      </c>
+      <c r="H70" s="4">
+        <f t="shared" si="1"/>
+        <v>7.2857142857142856</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>